<commit_message>
Update of Test cases - Sprint 5
Last version.
</commit_message>
<xml_diff>
--- a/Appetite - Test Cases - Sprint 5.xlsx
+++ b/Appetite - Test Cases - Sprint 5.xlsx
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>TC1</t>
   </si>
@@ -185,7 +185,7 @@
 </t>
   </si>
   <si>
-    <t>To be able to view price category for a choose restaurant.</t>
+    <t>To be able to view price category for a choose restaurant in the list and detail screens.</t>
   </si>
 </sst>
 </file>
@@ -904,6 +904,27 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -916,9 +937,6 @@
     <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="4" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -935,24 +953,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="4" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="19" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1309,7 +1309,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="D10" sqref="D10:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1332,15 +1332,15 @@
       <c r="A2" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="65"/>
-      <c r="C2" s="65"/>
-      <c r="D2" s="66"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="55"/>
       <c r="E2" s="39"/>
       <c r="F2" s="39"/>
       <c r="G2" s="39"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="67"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
       <c r="K2" s="40"/>
       <c r="L2" s="40"/>
     </row>
@@ -1361,9 +1361,9 @@
       <c r="E3" s="44"/>
       <c r="F3" s="44"/>
       <c r="G3" s="44"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
+      <c r="H3" s="57"/>
+      <c r="I3" s="57"/>
+      <c r="J3" s="57"/>
       <c r="K3" s="40"/>
       <c r="L3" s="40"/>
     </row>
@@ -1384,17 +1384,17 @@
       <c r="E4" s="49"/>
       <c r="F4" s="49"/>
       <c r="G4" s="49"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
       <c r="K4" s="40"/>
       <c r="L4" s="40"/>
     </row>
     <row r="5" spans="1:12" s="1" customFormat="1" ht="18">
-      <c r="A5" s="68"/>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="58"/>
+      <c r="D5" s="58"/>
       <c r="E5" s="44"/>
       <c r="F5" s="44"/>
       <c r="G5" s="44"/>
@@ -1405,46 +1405,46 @@
       <c r="L5" s="40"/>
     </row>
     <row r="6" spans="1:12" s="33" customFormat="1" ht="18">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="56" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="60"/>
-      <c r="F6" s="61"/>
-      <c r="G6" s="69" t="s">
+      <c r="E6" s="66"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="H6" s="58" t="s">
+      <c r="H6" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="58" t="s">
+      <c r="I6" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="58" t="s">
+      <c r="J6" s="56" t="s">
         <v>22</v>
       </c>
       <c r="K6" s="40"/>
       <c r="L6" s="40"/>
     </row>
     <row r="7" spans="1:12" s="27" customFormat="1" ht="18">
-      <c r="A7" s="58"/>
-      <c r="B7" s="57"/>
-      <c r="C7" s="58"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="70"/>
-      <c r="H7" s="58"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="58"/>
+      <c r="A7" s="56"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="56"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="60"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="56"/>
+      <c r="J7" s="56"/>
       <c r="K7" s="50"/>
       <c r="L7" s="50"/>
     </row>
@@ -1458,11 +1458,11 @@
       <c r="C8" s="51" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="54" t="s">
+      <c r="D8" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="55"/>
-      <c r="F8" s="56"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="63"/>
       <c r="G8" s="51" t="s">
         <v>34</v>
       </c>
@@ -1484,11 +1484,11 @@
       <c r="C9" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="54" t="s">
+      <c r="D9" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="55"/>
-      <c r="F9" s="56"/>
+      <c r="E9" s="62"/>
+      <c r="F9" s="63"/>
       <c r="G9" s="51" t="s">
         <v>28</v>
       </c>
@@ -1510,18 +1510,20 @@
       <c r="C10" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="54" t="s">
+      <c r="D10" s="61" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="55"/>
-      <c r="F10" s="56"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="63"/>
       <c r="G10" s="51" t="s">
         <v>39</v>
       </c>
       <c r="H10" s="52">
         <v>43186</v>
       </c>
-      <c r="I10" s="51"/>
+      <c r="I10" s="51" t="s">
+        <v>23</v>
+      </c>
       <c r="J10" s="51"/>
       <c r="K10" s="53"/>
       <c r="L10" s="53"/>
@@ -1536,11 +1538,11 @@
       <c r="C11" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="54" t="s">
+      <c r="D11" s="61" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="55"/>
-      <c r="F11" s="56"/>
+      <c r="E11" s="62"/>
+      <c r="F11" s="63"/>
       <c r="G11" s="51" t="s">
         <v>34</v>
       </c>
@@ -1554,6 +1556,14 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D6:F7"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D8:F8"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="H2:J2"/>
@@ -1563,14 +1573,6 @@
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="G6:G7"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D6:F7"/>
   </mergeCells>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Including Test Case for User Story #155644469
</commit_message>
<xml_diff>
--- a/Appetite - Test Cases - Sprint 5.xlsx
+++ b/Appetite - Test Cases - Sprint 5.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10210"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28615"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sergiodealmeidabrunacci/Mobile_Developer/Mobile Application Dev Project/Test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fernandoito/Documents/GitHub/726/Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="821"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="821"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint-5" sheetId="122" r:id="rId1"/>
@@ -28,12 +28,20 @@
     <definedName name="Port">[1]Validation!$F$2:$F$40</definedName>
     <definedName name="VancoProducts">[1]Validation!$B$2:$B$4</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="56">
   <si>
     <t>TC1</t>
   </si>
@@ -200,15 +208,32 @@
   <si>
     <t>To be able to view price category for a choose restaurant in the detail screen.</t>
   </si>
+  <si>
+    <t xml:space="preserve">Open the list of restaurants from the menu at the top-right corner
+</t>
+  </si>
+  <si>
+    <t>Fernando</t>
+  </si>
+  <si>
+    <t>TC7</t>
+  </si>
+  <si>
+    <t>List Details
+Check if restaurant review appears in the list</t>
+  </si>
+  <si>
+    <t>For each restaurant listed you might see the restaurant review represented as the quantity of reviews and the text "reviews". For example, if the restaurant has 13 reviews, a grey text will appear on the left of the stars rate as "13 reviews".</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -345,279 +370,279 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="hair">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -626,75 +651,75 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -703,18 +728,18 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -722,7 +747,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -731,7 +756,7 @@
       <left/>
       <right/>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -739,10 +764,10 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
@@ -880,6 +905,12 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -889,15 +920,30 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="21" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="22" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -908,27 +954,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="25" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="23" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="30" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="24" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="26" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="27" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3291,9 +3316,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -3321,31 +3346,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -3373,23 +3381,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3566,16 +3557,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
+  <sheetPr enableFormatConditionsCalculation="0">
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.33203125" style="39" customWidth="1"/>
@@ -3584,32 +3575,31 @@
     <col min="6" max="6" width="27.83203125" customWidth="1"/>
     <col min="7" max="7" width="18.5" customWidth="1"/>
     <col min="8" max="8" width="17.1640625" customWidth="1"/>
-    <col min="9" max="9" width="9" style="8"/>
+    <col min="9" max="9" width="8.83203125" style="8"/>
     <col min="10" max="10" width="18" style="42" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15" thickBot="1"/>
-    <row r="2" spans="1:10" s="1" customFormat="1">
+    <row r="1" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="55"/>
+      <c r="B2" s="62"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="63"/>
       <c r="E2" s="29"/>
       <c r="F2" s="29"/>
       <c r="G2" s="29"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
     </row>
-    <row r="3" spans="1:10" s="1" customFormat="1" ht="13">
+    <row r="3" spans="1:10" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="43" t="s">
         <v>24</v>
       </c>
       <c r="B3" s="44">
-        <f>COUNTIF(I8:I12,"Pass")</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" s="44" t="s">
         <v>25</v>
@@ -3621,11 +3611,11 @@
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
     </row>
-    <row r="4" spans="1:10" s="1" customFormat="1" thickBot="1">
+    <row r="4" spans="1:10" s="1" customFormat="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A4" s="46" t="s">
         <v>4</v>
       </c>
@@ -3637,21 +3627,20 @@
         <v>19</v>
       </c>
       <c r="D4" s="48">
-        <f>COUNTA(A8:A12)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E4" s="30"/>
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
     </row>
-    <row r="5" spans="1:10" s="1" customFormat="1" ht="13">
-      <c r="A5" s="58"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
+    <row r="5" spans="1:10" s="1" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A5" s="65"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
@@ -3659,47 +3648,47 @@
       <c r="I5" s="41"/>
       <c r="J5" s="41"/>
     </row>
-    <row r="6" spans="1:10" s="37" customFormat="1" ht="15">
-      <c r="A6" s="56" t="s">
+    <row r="6" spans="1:10" s="37" customFormat="1" ht="15" x14ac:dyDescent="0.15">
+      <c r="A6" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="56" t="s">
+      <c r="C6" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="62" t="s">
+      <c r="D6" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="63"/>
-      <c r="F6" s="64"/>
-      <c r="G6" s="59" t="s">
+      <c r="E6" s="57"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="H6" s="56" t="s">
+      <c r="H6" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="56" t="s">
+      <c r="I6" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="56" t="s">
+      <c r="J6" s="52" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="31" customFormat="1" ht="13">
-      <c r="A7" s="56"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="56"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="56"/>
-      <c r="I7" s="56"/>
-      <c r="J7" s="56"/>
+    <row r="7" spans="1:10" s="31" customFormat="1" ht="13" x14ac:dyDescent="0.15">
+      <c r="A7" s="52"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="52"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
     </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" ht="26">
+    <row r="8" spans="1:10" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="38" t="s">
         <v>0</v>
       </c>
@@ -3709,11 +3698,11 @@
       <c r="C8" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="51" t="s">
+      <c r="D8" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="52"/>
-      <c r="F8" s="53"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="55"/>
       <c r="G8" s="38" t="s">
         <v>27</v>
       </c>
@@ -3725,7 +3714,7 @@
       </c>
       <c r="J8" s="38"/>
     </row>
-    <row r="9" spans="1:10" s="2" customFormat="1" ht="26">
+    <row r="9" spans="1:10" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="38" t="s">
         <v>1</v>
       </c>
@@ -3735,11 +3724,11 @@
       <c r="C9" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="52"/>
-      <c r="F9" s="53"/>
+      <c r="E9" s="54"/>
+      <c r="F9" s="55"/>
       <c r="G9" s="38" t="s">
         <v>27</v>
       </c>
@@ -3751,7 +3740,7 @@
       </c>
       <c r="J9" s="38"/>
     </row>
-    <row r="10" spans="1:10" s="2" customFormat="1" ht="26">
+    <row r="10" spans="1:10" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="38" t="s">
         <v>2</v>
       </c>
@@ -3761,11 +3750,11 @@
       <c r="C10" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="D10" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="52"/>
-      <c r="F10" s="53"/>
+      <c r="E10" s="54"/>
+      <c r="F10" s="55"/>
       <c r="G10" s="38" t="s">
         <v>27</v>
       </c>
@@ -3777,7 +3766,7 @@
       </c>
       <c r="J10" s="38"/>
     </row>
-    <row r="11" spans="1:10" s="2" customFormat="1" ht="85.75" customHeight="1">
+    <row r="11" spans="1:10" s="2" customFormat="1" ht="85.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="38" t="s">
         <v>3</v>
       </c>
@@ -3787,11 +3776,11 @@
       <c r="C11" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="51" t="s">
+      <c r="D11" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="E11" s="52"/>
-      <c r="F11" s="53"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="55"/>
       <c r="G11" s="38" t="s">
         <v>27</v>
       </c>
@@ -3803,7 +3792,7 @@
       </c>
       <c r="J11" s="38"/>
     </row>
-    <row r="12" spans="1:10" ht="43" customHeight="1">
+    <row r="12" spans="1:10" ht="43" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="38" t="s">
         <v>41</v>
       </c>
@@ -3813,11 +3802,11 @@
       <c r="C12" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="52"/>
-      <c r="F12" s="53"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="55"/>
       <c r="G12" s="38" t="s">
         <v>42</v>
       </c>
@@ -3829,7 +3818,7 @@
       </c>
       <c r="J12" s="38"/>
     </row>
-    <row r="13" spans="1:10" ht="43" customHeight="1">
+    <row r="13" spans="1:10" ht="43" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="38" t="s">
         <v>44</v>
       </c>
@@ -3839,11 +3828,11 @@
       <c r="C13" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="D13" s="51" t="s">
+      <c r="D13" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="52"/>
-      <c r="F13" s="53"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="55"/>
       <c r="G13" s="38" t="s">
         <v>42</v>
       </c>
@@ -3855,14 +3844,39 @@
       </c>
       <c r="J13" s="38"/>
     </row>
+    <row r="14" spans="1:10" ht="41" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="53" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="54"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="J14" s="38"/>
+    </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D11:F11"/>
-    <mergeCell ref="D6:F7"/>
+  <mergeCells count="20">
+    <mergeCell ref="D12:F12"/>
+    <mergeCell ref="D13:F13"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="D14:F14"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="H2:J2"/>
@@ -3872,10 +3886,12 @@
     <mergeCell ref="H3:J3"/>
     <mergeCell ref="H4:J4"/>
     <mergeCell ref="G6:G7"/>
-    <mergeCell ref="D12:F12"/>
-    <mergeCell ref="D13:F13"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D6:F7"/>
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3892,13 +3908,13 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="22.83203125" customWidth="1"/>
     <col min="7" max="7" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="23">
+    <row r="1" spans="1:7" ht="23" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3909,7 +3925,7 @@
       <c r="F1" s="6"/>
       <c r="G1" s="7"/>
     </row>
-    <row r="2" spans="1:7" ht="14.25" customHeight="1">
+    <row r="2" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="5"/>
       <c r="C2" s="6"/>
@@ -3918,7 +3934,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="7"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B3" s="8" t="s">
         <v>8</v>
       </c>
@@ -3928,7 +3944,7 @@
       <c r="F3" s="6"/>
       <c r="G3" s="7"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="B4" s="8" t="s">
         <v>5</v>
       </c>
@@ -3938,7 +3954,7 @@
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -3947,7 +3963,7 @@
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -3956,7 +3972,7 @@
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" spans="1:7" ht="26">
+    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="9"/>
       <c r="B7" s="19" t="s">
         <v>11</v>
@@ -3977,7 +3993,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="28" customFormat="1">
+    <row r="8" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A8" s="32"/>
       <c r="B8" s="33">
         <v>1</v>
@@ -3987,7 +4003,7 @@
       </c>
       <c r="D8" s="35">
         <f>'Sprint-5'!B3</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E8" s="34">
         <f>'Sprint-5'!B4</f>
@@ -3999,10 +4015,10 @@
       </c>
       <c r="G8" s="35">
         <f>'Sprint-5'!D4</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="8"/>
       <c r="B9" s="17"/>
       <c r="C9" s="16"/>
@@ -4011,7 +4027,7 @@
       <c r="F9" s="15"/>
       <c r="G9" s="18"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="8"/>
       <c r="B10" s="23"/>
       <c r="C10" s="24" t="s">
@@ -4019,7 +4035,7 @@
       </c>
       <c r="D10" s="25">
         <f>SUM(D6:D9)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E10" s="25">
         <f>SUM(E6:E9)</f>
@@ -4031,10 +4047,10 @@
       </c>
       <c r="G10" s="26">
         <f>SUM(G6:G9)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="8"/>
       <c r="B11" s="10"/>
       <c r="C11" s="8"/>
@@ -4043,7 +4059,7 @@
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="8"/>
       <c r="B12" s="8"/>
       <c r="C12" s="8" t="s">
@@ -4059,7 +4075,7 @@
       </c>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="8"/>
       <c r="B13" s="8"/>
       <c r="C13" s="8" t="s">

</xml_diff>